<commit_message>
fix: only complain about ambiguous headers if they're used
If the ambiguous headers are in a file, but they're not referenced,
no reason to care about them
</commit_message>
<xml_diff>
--- a/resources/fixtures/products.xlsx
+++ b/resources/fixtures/products.xlsx
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
   <si>
     <t xml:space="preserve">Price USD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duplicate</t>
   </si>
   <si>
     <t xml:space="preserve">The Very Hungry Caterpillar</t>
@@ -154,12 +157,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -169,10 +172,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -189,29 +192,53 @@
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>